<commit_message>
✅ Cambios recientes en principal.py
</commit_message>
<xml_diff>
--- a/indicadores.xlsx
+++ b/indicadores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29103"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgonzalezf\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1735" documentId="13_ncr:1_{F9A0C0D9-DCE9-49D4-A175-8E88C99C35D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{885D0009-69A1-46E6-AB99-7BA086BA873E}"/>
+  <xr:revisionPtr revIDLastSave="1746" documentId="13_ncr:1_{F9A0C0D9-DCE9-49D4-A175-8E88C99C35D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E5F53D3-9339-4183-81A3-C9562494823B}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65C7F682-817E-4853-A611-DB14C5FF8504}"/>
   </bookViews>
@@ -977,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5A7E77-A627-48E3-86E5-02689C5AE68E}">
   <dimension ref="B1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.6"/>
@@ -1012,8 +1012,8 @@
         <v>2</v>
       </c>
       <c r="E3" s="35">
-        <f>10+15+4+5</f>
-        <v>34</v>
+        <f>10+15+4+5-5</f>
+        <v>29</v>
       </c>
       <c r="F3" s="36" t="s">
         <v>2</v>
@@ -1028,8 +1028,8 @@
         <v>3</v>
       </c>
       <c r="E4" s="45">
-        <f>12+6</f>
-        <v>18</v>
+        <f>12+6+5</f>
+        <v>23</v>
       </c>
       <c r="F4" s="46" t="s">
         <v>3</v>
@@ -1047,8 +1047,8 @@
         <v>4</v>
       </c>
       <c r="F5" s="42">
-        <f>16/43</f>
-        <v>0.37209302325581395</v>
+        <f>21/43</f>
+        <v>0.48837209302325579</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="12.75">
@@ -1056,13 +1056,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="39">
-        <v>2.8400000000000002E-2</v>
+        <v>9.1899999999999996E-2</v>
       </c>
       <c r="E6" s="37" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="39">
-        <v>3.0300000000000001E-2</v>
+        <v>9.7000000000000003E-2</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="12.75">
@@ -1260,7 +1260,7 @@
         <v>20</v>
       </c>
       <c r="F20" s="44">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="12.75">
@@ -2120,7 +2120,7 @@
       <c r="A3" s="6"/>
       <c r="B3" s="47">
         <f>'ÁREA GESTIÓN CORPORATIVA'!B3+'ÁREA GESTIÓN CORPORATIVA'!E3+'ÁREA TECH'!B3+'ÁREA TECH'!E3+'ÁREA TECH'!B27+'ÁREA TECH'!E27</f>
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="C3" s="56" t="s">
         <v>49</v>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="C4" s="55">
         <f>('ÁREA GESTIÓN CORPORATIVA'!C5+'ÁREA GESTIÓN CORPORATIVA'!F5+'ÁREA TECH'!C5+'ÁREA TECH'!F5+'ÁREA TECH'!C28+'ÁREA TECH'!F28)/6</f>
-        <v>0.3741408861389659</v>
+        <v>0.39352073110020624</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="7" t="s">
@@ -2159,7 +2159,7 @@
       </c>
       <c r="C5" s="9">
         <f>('ÁREA GESTIÓN CORPORATIVA'!C6+'ÁREA GESTIÓN CORPORATIVA'!F6+'ÁREA TECH'!C6+'ÁREA TECH'!F6+'ÁREA TECH'!C29+'ÁREA TECH'!F29)/6</f>
-        <v>6.6549999999999998E-2</v>
+        <v>8.8250000000000009E-2</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="7" t="s">
@@ -2417,17 +2417,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="dd16a1b9-1647-43af-9f4a-98401eda4351" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c20bc9ba-56db-4433-b77e-d60cd7e78f68">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101000A8D16C3BDDAC448857F64EC1B88B6E8" ma:contentTypeVersion="16" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fa096be39ecaf3f9d6ded1545869b31a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c20bc9ba-56db-4433-b77e-d60cd7e78f68" xmlns:ns3="dd16a1b9-1647-43af-9f4a-98401eda4351" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d9952885a40765fe2073c79b04c2cf4" ns2:_="" ns3:_="">
     <xsd:import namespace="c20bc9ba-56db-4433-b77e-d60cd7e78f68"/>
@@ -2668,14 +2657,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="dd16a1b9-1647-43af-9f4a-98401eda4351" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c20bc9ba-56db-4433-b77e-d60cd7e78f68">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC7512B-2F85-4D86-B3D0-845A2A245CB3}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AF193F7-71C7-4303-9B87-3BF8D09271BC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{007C5A0E-91F4-4F27-825F-68E1BE16310D}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{007C5A0E-91F4-4F27-825F-68E1BE16310D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AF193F7-71C7-4303-9B87-3BF8D09271BC}"/>
 </file>
</xml_diff>

<commit_message>
feat(streamlit): botón recargar caché + limpieza tablas/consultores + parser fechas ES
</commit_message>
<xml_diff>
--- a/indicadores.xlsx
+++ b/indicadores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29122"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgonzalezf\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1746" documentId="13_ncr:1_{F9A0C0D9-DCE9-49D4-A175-8E88C99C35D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E5F53D3-9339-4183-81A3-C9562494823B}"/>
+  <xr:revisionPtr revIDLastSave="1769" documentId="13_ncr:1_{F9A0C0D9-DCE9-49D4-A175-8E88C99C35D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05615BCA-2A66-4082-AC04-542A19DAA7F4}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65C7F682-817E-4853-A611-DB14C5FF8504}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{65C7F682-817E-4853-A611-DB14C5FF8504}"/>
   </bookViews>
   <sheets>
     <sheet name="ÁREA GESTIÓN CORPORATIVA" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="59">
   <si>
     <t xml:space="preserve">Máster Profesional en RRHH: </t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>Certificación SAP:</t>
+  </si>
+  <si>
+    <t>21 ALUMNOS</t>
   </si>
   <si>
     <t>Recomendación docente alumnado</t>
@@ -977,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5A7E77-A627-48E3-86E5-02689C5AE68E}">
   <dimension ref="B1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.6"/>
@@ -1319,8 +1322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D220AC93-A43D-439D-85C7-CB935101DEDC}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1772,7 +1775,7 @@
         <v>41</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="G25" s="5"/>
     </row>
@@ -1803,7 +1806,7 @@
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="19">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F27" s="31" t="s">
         <v>32</v>
@@ -1823,7 +1826,7 @@
         <v>4</v>
       </c>
       <c r="F28" s="25">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="G28" s="5"/>
     </row>
@@ -1840,7 +1843,7 @@
         <v>5</v>
       </c>
       <c r="F29" s="24">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="5"/>
     </row>
@@ -1857,7 +1860,7 @@
         <v>6</v>
       </c>
       <c r="F30" s="24">
-        <v>0.1429</v>
+        <v>0</v>
       </c>
       <c r="G30" s="5"/>
     </row>
@@ -1908,7 +1911,7 @@
         <v>9</v>
       </c>
       <c r="F33" s="25">
-        <v>0.57999999999999996</v>
+        <v>0</v>
       </c>
       <c r="G33" s="5"/>
     </row>
@@ -1925,7 +1928,7 @@
         <v>10</v>
       </c>
       <c r="F34" s="24">
-        <v>0.91</v>
+        <v>0.89</v>
       </c>
       <c r="G34" s="5"/>
     </row>
@@ -1941,25 +1944,23 @@
       <c r="E35" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="24">
-        <v>0.46</v>
-      </c>
+      <c r="F35" s="24"/>
       <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="5"/>
       <c r="B36" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C36" s="51">
         <v>0</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F36" s="51">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G36" s="5"/>
     </row>
@@ -2004,12 +2005,12 @@
         <v>15</v>
       </c>
       <c r="F39" s="44">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="B40" s="37" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C40" s="67">
         <v>0</v>
@@ -2018,7 +2019,7 @@
         <v>16</v>
       </c>
       <c r="F40" s="44">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2032,21 +2033,21 @@
         <v>17</v>
       </c>
       <c r="F41" s="44">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="B42" s="37" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C42" s="67">
         <v>0</v>
       </c>
       <c r="E42" s="37" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F42" s="44">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2058,12 +2059,12 @@
         <v>23</v>
       </c>
       <c r="F43" s="44">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="B44" s="77" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C44" s="78">
         <v>0</v>
@@ -2107,12 +2108,12 @@
     <row r="2" spans="1:6">
       <c r="A2" s="6"/>
       <c r="B2" s="82" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" s="83"/>
       <c r="D2" s="6"/>
       <c r="E2" s="82" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" s="83"/>
     </row>
@@ -2120,14 +2121,14 @@
       <c r="A3" s="6"/>
       <c r="B3" s="47">
         <f>'ÁREA GESTIÓN CORPORATIVA'!B3+'ÁREA GESTIÓN CORPORATIVA'!E3+'ÁREA TECH'!B3+'ÁREA TECH'!E3+'ÁREA TECH'!B27+'ÁREA TECH'!E27</f>
-        <v>353</v>
+        <v>324</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F3" s="63">
         <v>62498.559999999998</v>
@@ -2141,11 +2142,11 @@
       </c>
       <c r="C4" s="55">
         <f>('ÁREA GESTIÓN CORPORATIVA'!C5+'ÁREA GESTIÓN CORPORATIVA'!F5+'ÁREA TECH'!C5+'ÁREA TECH'!F5+'ÁREA TECH'!C28+'ÁREA TECH'!F28)/6</f>
-        <v>0.39352073110020624</v>
+        <v>0.41852073110020621</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F4" s="13">
         <v>66</v>
@@ -2159,11 +2160,11 @@
       </c>
       <c r="C5" s="9">
         <f>('ÁREA GESTIÓN CORPORATIVA'!C6+'ÁREA GESTIÓN CORPORATIVA'!F6+'ÁREA TECH'!C6+'ÁREA TECH'!F6+'ÁREA TECH'!C29+'ÁREA TECH'!F29)/6</f>
-        <v>8.8250000000000009E-2</v>
+        <v>7.1583333333333346E-2</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F5" s="13">
         <v>105</v>
@@ -2177,11 +2178,11 @@
       </c>
       <c r="C6" s="9">
         <f>('ÁREA GESTIÓN CORPORATIVA'!C7+'ÁREA GESTIÓN CORPORATIVA'!F7+'ÁREA TECH'!C7+'ÁREA TECH'!F7+'ÁREA TECH'!C30+'ÁREA TECH'!F30)/6</f>
-        <v>7.1233333333333329E-2</v>
+        <v>4.7416666666666663E-2</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F6" s="14">
         <v>18508.82</v>
@@ -2231,7 +2232,7 @@
       </c>
       <c r="C10" s="9">
         <f>('ÁREA GESTIÓN CORPORATIVA'!C11+'ÁREA GESTIÓN CORPORATIVA'!F11+'ÁREA TECH'!C11+'ÁREA TECH'!F11+'ÁREA TECH'!C34+'ÁREA TECH'!F34)/6</f>
-        <v>0.8580000000000001</v>
+        <v>0.85466666666666669</v>
       </c>
       <c r="D10" s="6"/>
     </row>
@@ -2243,7 +2244,7 @@
       </c>
       <c r="C11" s="9">
         <f>('ÁREA TECH'!C35+'ÁREA TECH'!F35+'ÁREA TECH'!C12+'ÁREA TECH'!F12+'ÁREA GESTIÓN CORPORATIVA'!C12+'ÁREA GESTIÓN CORPORATIVA'!F12)/6</f>
-        <v>0.15757693413862525</v>
+        <v>8.0910267471958577E-2</v>
       </c>
       <c r="D11" s="6"/>
     </row>
@@ -2255,7 +2256,7 @@
       </c>
       <c r="C12" s="54">
         <f>'ÁREA GESTIÓN CORPORATIVA'!C13+'ÁREA GESTIÓN CORPORATIVA'!F13+'ÁREA TECH'!C13+'ÁREA TECH'!F13+'ÁREA TECH'!F36+'ÁREA TECH'!C36</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" s="6"/>
     </row>
@@ -2278,7 +2279,7 @@
       </c>
       <c r="C15" s="66">
         <f>SUM(C16:C28)</f>
-        <v>502</v>
+        <v>449</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1">
@@ -2287,7 +2288,7 @@
       </c>
       <c r="C16" s="13">
         <f>'ÁREA GESTIÓN CORPORATIVA'!C16+'ÁREA GESTIÓN CORPORATIVA'!F16+'ÁREA TECH'!C39+'ÁREA TECH'!F39+'ÁREA TECH'!C16+'ÁREA TECH'!F16</f>
-        <v>297</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="15" customHeight="1">
@@ -2296,7 +2297,7 @@
       </c>
       <c r="C17" s="13">
         <f>'ÁREA GESTIÓN CORPORATIVA'!C17+'ÁREA GESTIÓN CORPORATIVA'!F17++'ÁREA TECH'!F17+'ÁREA TECH'!C43+'ÁREA TECH'!F40</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="15" customHeight="1">
@@ -2305,7 +2306,7 @@
       </c>
       <c r="C18" s="13">
         <f>'ÁREA GESTIÓN CORPORATIVA'!C18+'ÁREA GESTIÓN CORPORATIVA'!F18+'ÁREA TECH'!C18+'ÁREA TECH'!F18+'ÁREA TECH'!C41+'ÁREA TECH'!F41</f>
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="15" customHeight="1">
@@ -2328,7 +2329,7 @@
     </row>
     <row r="21" spans="2:3" ht="15" customHeight="1">
       <c r="B21" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C21" s="13">
         <f>'ÁREA TECH'!C19</f>
@@ -2364,7 +2365,7 @@
     </row>
     <row r="25" spans="2:3" ht="15" customHeight="1">
       <c r="B25" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C25" s="13">
         <f>'ÁREA TECH'!F22</f>
@@ -2373,7 +2374,7 @@
     </row>
     <row r="26" spans="2:3" ht="15" customHeight="1">
       <c r="B26" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C26" s="13">
         <f>'ÁREA TECH'!C42</f>
@@ -2382,20 +2383,20 @@
     </row>
     <row r="27" spans="2:3" ht="15" customHeight="1">
       <c r="B27" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C27" s="13">
         <f>'ÁREA TECH'!F42</f>
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="15" customHeight="1">
       <c r="B28" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C28" s="59">
         <f>'ÁREA TECH'!F43</f>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2408,12 +2409,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="dd16a1b9-1647-43af-9f4a-98401eda4351" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c20bc9ba-56db-4433-b77e-d60cd7e78f68">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2658,18 +2661,16 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="dd16a1b9-1647-43af-9f4a-98401eda4351" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c20bc9ba-56db-4433-b77e-d60cd7e78f68">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC7512B-2F85-4D86-B3D0-845A2A245CB3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AF193F7-71C7-4303-9B87-3BF8D09271BC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2677,5 +2678,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AF193F7-71C7-4303-9B87-3BF8D09271BC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC7512B-2F85-4D86-B3D0-845A2A245CB3}"/>
 </file>
</xml_diff>